<commit_message>
Update period list to log space
</commit_message>
<xml_diff>
--- a/sample/Matching-Assessment/data/output_files/output_matching_assessment.xlsx
+++ b/sample/Matching-Assessment/data/output_files/output_matching_assessment.xlsx
@@ -759,7 +759,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -845,407 +845,3452 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.075</v>
+        <v>0.01059766248676071</v>
       </c>
       <c r="B3" t="n">
-        <v>0.585070268206077</v>
+        <v>0.4218975627149371</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4370596175291448</v>
+        <v>0.3713891527747594</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4332358995653619</v>
+        <v>0.4027534239760137</v>
       </c>
       <c r="E3" t="n">
-        <v>0.439038585215055</v>
+        <v>0.3757742623548179</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6467588668706312</v>
+        <v>0.4709344357726963</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6814559806833883</v>
+        <v>0.415596657565434</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4405176529606186</v>
+        <v>0.425368232569704</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5137257514817218</v>
+        <v>0.4107982441736384</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.1</v>
+        <v>0.01123104501832952</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8852589998519819</v>
+        <v>0.4219398849210421</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5803119452305643</v>
+        <v>0.3685581394982932</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5127388794768729</v>
+        <v>0.4015208519617428</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5649230309439258</v>
+        <v>0.371300462857554</v>
       </c>
       <c r="F4" t="n">
-        <v>0.70912717261294</v>
+        <v>0.4655459787152564</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8443216012261132</v>
+        <v>0.413082158375949</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5013595896681875</v>
+        <v>0.4243181750692611</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6414202664842646</v>
+        <v>0.4083033810604067</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.15</v>
+        <v>0.01190228244778715</v>
       </c>
       <c r="B5" t="n">
-        <v>1.197686193209774</v>
+        <v>0.4220797037975347</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7255498690222324</v>
+        <v>0.3696423970755814</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6163123340372031</v>
+        <v>0.4013042618481464</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9307589190115891</v>
+        <v>0.3720414437763533</v>
       </c>
       <c r="F5" t="n">
-        <v>0.779436493468399</v>
+        <v>0.4584339186949194</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6982669833336945</v>
+        <v>0.4099784780627973</v>
       </c>
       <c r="H5" t="n">
-        <v>0.5932405078561168</v>
+        <v>0.4250098941849249</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7703157436260021</v>
+        <v>0.4073371552320552</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.2</v>
+        <v>0.01261363722037444</v>
       </c>
       <c r="B6" t="n">
-        <v>1.091566373328303</v>
+        <v>0.4220616235021325</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9451668916946664</v>
+        <v>0.3701596926874079</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7490450417414459</v>
+        <v>0.4016593015903909</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8619664758137654</v>
+        <v>0.371886500935032</v>
       </c>
       <c r="F6" t="n">
-        <v>1.020155928251652</v>
+        <v>0.4648082653197225</v>
       </c>
       <c r="G6" t="n">
-        <v>1.015059898966836</v>
+        <v>0.4097787545931046</v>
       </c>
       <c r="H6" t="n">
-        <v>0.7762783233148871</v>
+        <v>0.4255699787918944</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9146343774387705</v>
+        <v>0.4082962177737381</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.3</v>
+        <v>0.01336750699919708</v>
       </c>
       <c r="B7" t="n">
-        <v>1.07351993569096</v>
+        <v>0.4221258847930199</v>
       </c>
       <c r="C7" t="n">
-        <v>1.041982983664943</v>
+        <v>0.3704512180012256</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8690271890399308</v>
+        <v>0.4016447688916768</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9286762308014523</v>
+        <v>0.373267916413862</v>
       </c>
       <c r="F7" t="n">
-        <v>1.09272102269251</v>
+        <v>0.4714269293269746</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9282350840413457</v>
+        <v>0.4111244140316297</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9369205965507144</v>
+        <v>0.4267863999054532</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9783431624790606</v>
+        <v>0.4097501723895079</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.5</v>
+        <v>0.01416643274669021</v>
       </c>
       <c r="B8" t="n">
-        <v>1.24096674832894</v>
+        <v>0.4222433600342306</v>
       </c>
       <c r="C8" t="n">
-        <v>1.142177881407323</v>
+        <v>0.3707981044949409</v>
       </c>
       <c r="D8" t="n">
-        <v>1.049369764593732</v>
+        <v>0.4030452604825234</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9326073413632268</v>
+        <v>0.3743846002696512</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9508858665102252</v>
+        <v>0.4718726817389221</v>
       </c>
       <c r="G8" t="n">
-        <v>1.004172884877545</v>
+        <v>0.4131284949677801</v>
       </c>
       <c r="H8" t="n">
-        <v>1.176796076753402</v>
+        <v>0.428213436232923</v>
       </c>
       <c r="I8" t="n">
-        <v>1.065459758973728</v>
+        <v>0.410736408026579</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.75</v>
+        <v>0.01501310728908174</v>
       </c>
       <c r="B9" t="n">
-        <v>1.000204120000045</v>
+        <v>0.422371975973813</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9515935809302553</v>
+        <v>0.3713350674848986</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9218940972731196</v>
+        <v>0.4037428300207959</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8857925086030589</v>
+        <v>0.3748148552855396</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9177281607060006</v>
+        <v>0.4695220877402866</v>
       </c>
       <c r="G9" t="n">
-        <v>0.8951336418758253</v>
+        <v>0.4132301616202398</v>
       </c>
       <c r="H9" t="n">
-        <v>1.152596986165</v>
+        <v>0.4287297671474045</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9571413644602141</v>
+        <v>0.4108001773052959</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1</v>
+        <v>0.01591038439272153</v>
       </c>
       <c r="B10" t="n">
-        <v>0.8948795841621183</v>
+        <v>0.4225066601708885</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8322283420242896</v>
+        <v>0.3715909923547574</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8549997427805686</v>
+        <v>0.4040769887334105</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8967648517284827</v>
+        <v>0.3759363003895157</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8065138675031739</v>
+        <v>0.468292596533666</v>
       </c>
       <c r="G10" t="n">
-        <v>0.7939465373544355</v>
+        <v>0.4134602574966668</v>
       </c>
       <c r="H10" t="n">
-        <v>1.078844069218974</v>
+        <v>0.4295382146418183</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8755634712397024</v>
+        <v>0.411072637924096</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>0.0168612883828688</v>
       </c>
       <c r="B11" t="n">
-        <v>0.5129180019903586</v>
+        <v>0.4226277141280566</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3821839604694264</v>
+        <v>0.3718128105055785</v>
       </c>
       <c r="D11" t="n">
-        <v>0.37182821454383</v>
+        <v>0.4042633931558878</v>
       </c>
       <c r="E11" t="n">
-        <v>0.3309474841071652</v>
+        <v>0.376856279344724</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3937626936743817</v>
+        <v>0.4698159158800247</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3940310973711876</v>
+        <v>0.4137887836215572</v>
       </c>
       <c r="H11" t="n">
-        <v>0.3841372236389816</v>
+        <v>0.4311583771539115</v>
       </c>
       <c r="I11" t="n">
-        <v>0.3926027398080856</v>
+        <v>0.4117541320599099</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>3</v>
+        <v>0.01786902433735828</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2341730608383406</v>
+        <v>0.4227408015523108</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2106340255091969</v>
+        <v>0.3723240067406429</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2314584958672017</v>
+        <v>0.4053536256328614</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2175901157523291</v>
+        <v>0.3778263914426053</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2443153596965293</v>
+        <v>0.4711382047473844</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2600365810992653</v>
+        <v>0.4140708175582704</v>
       </c>
       <c r="H12" t="n">
-        <v>0.225448431407594</v>
+        <v>0.4281464986848847</v>
       </c>
       <c r="I12" t="n">
-        <v>0.2314507530264379</v>
+        <v>0.4119534353123442</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4</v>
+        <v>0.0189369888895036</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1649492267713028</v>
+        <v>0.4228589614174438</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1883481942698003</v>
+        <v>0.3726571073981049</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1830605636445518</v>
+        <v>0.4041229207747422</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1745526954833821</v>
+        <v>0.3785500078091939</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1756474558140235</v>
+        <v>0.4706131604375284</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1811435699832432</v>
+        <v>0.415076592338649</v>
       </c>
       <c r="H13" t="n">
-        <v>0.2253687193995513</v>
+        <v>0.4247398411668517</v>
       </c>
       <c r="I13" t="n">
-        <v>0.183919323329651</v>
+        <v>0.4115633697219195</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>5</v>
+        <v>0.02006878167664967</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1761762188765484</v>
+        <v>0.4229462198482662</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1431985069253469</v>
+        <v>0.3731598391919482</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1474359244538065</v>
+        <v>0.4053561462936662</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1601170733296252</v>
+        <v>0.3792169871058478</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1499943796110293</v>
+        <v>0.4705989078122371</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1838087331145352</v>
+        <v>0.4158473543980679</v>
       </c>
       <c r="H14" t="n">
-        <v>0.1887544718887741</v>
+        <v>0.4262420616486963</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1633194366537048</v>
+        <v>0.4122528615906615</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>7.5</v>
+        <v>0.02126821747296209</v>
       </c>
       <c r="B15" t="n">
-        <v>0.07077964193043591</v>
+        <v>0.4230428762983856</v>
       </c>
       <c r="C15" t="n">
-        <v>0.07044275250194941</v>
+        <v>0.3736808691160781</v>
       </c>
       <c r="D15" t="n">
-        <v>0.08968456684705818</v>
+        <v>0.4064982545923876</v>
       </c>
       <c r="E15" t="n">
-        <v>0.08042368238972805</v>
+        <v>0.3799502504458869</v>
       </c>
       <c r="F15" t="n">
-        <v>0.09911743194559385</v>
+        <v>0.469974219602419</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1295750976975764</v>
+        <v>0.4165932210421309</v>
       </c>
       <c r="H15" t="n">
-        <v>0.07285852580991359</v>
+        <v>0.4281614670533675</v>
       </c>
       <c r="I15" t="n">
-        <v>0.08559104534528569</v>
+        <v>0.4129204148343542</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
+        <v>0.02253933904734791</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.4231872074689114</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.3740385851154733</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.4039215791030513</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.3807868608789221</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.4682893912489389</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.4180369372978891</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.4226817994179173</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.4119850870459564</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0.02388643078984598</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.4233325344560515</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.3747220265055313</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.4076025840983064</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.3820659562006394</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.4711812738159502</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.4180285973337449</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.416991329852941</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.4124076758336137</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0.02531403315241567</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.4234930787658279</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.3755212626962635</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.4062201728028621</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.3833248551166492</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.4756107905931498</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.4197677288119701</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.4177365741116201</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.4134515762498452</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>0.02682695795279726</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.4236834975740314</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.3755091573005467</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.4062654202202715</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.3846973704844895</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.4736137114925682</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.4194871263616398</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.4215390998530812</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.4139413831318681</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0.02843030459302663</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.4239071828810042</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.3758920799079897</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.4077798394556404</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.386737705369252</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.4725932484171296</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.4175039264551191</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.4229291353694782</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.4143527936383801</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0.03012947724726992</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.4241556391262562</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.3765412901019334</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.4086396648634951</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.3889786661825139</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.4737675962787369</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.4223872555349877</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.420932274103781</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.4155130310609471</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>0.03193020307691027</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.4244031929127015</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.3780325877202906</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.4083900260860137</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.3901980436266462</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.4818210453114883</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.4214921719951353</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.4188098777061516</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.4165075696507817</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>0.03383855153428234</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.424680154408536</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.3791206418484205</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.4094139745196022</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.3894904848029622</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.4681772062834913</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.4182065995535396</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.4212967741038607</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.4149387818864129</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>0.03586095482011831</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.4249612236479041</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.3798923686051844</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.4128302167725472</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.3904835006829709</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.4779920681912115</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.4278340301028989</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.4252548961912962</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.4188940548992752</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0.03800422956365886</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.4252619913846727</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.3797262850654913</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.4135723491043068</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.3943575696243111</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.4802912842764062</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.4641187245529023</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.4272025890116656</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.4250858550699469</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>0.04027559979850297</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.4256718632792384</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.3809472807116217</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.425251504190954</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.3982370533184912</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.4717449060196079</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.4513765974690963</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.4261453740793078</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.42469379113466</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>0.04268272131163822</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.4263027442236264</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.3861899751121529</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.4198122293669188</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.401596565143694</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.5033761805505543</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.4863330903905927</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.4257422861854265</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.4338443281930648</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>0.04523370744772101</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.4270542745746828</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.385154948218731</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.4241639790904004</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.4088174492484054</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.5597377515950592</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.4633418942359904</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.4286391478355089</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.4395647154249933</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>0.04793715645558216</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.4278573073162567</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.3860010811481399</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.413584827931254</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.4106120975028744</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.5506705923682845</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.4879035554297817</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.4338029860079003</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.4414836277661774</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>0.05080218046913023</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.4369153797164265</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.3880195391866584</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.4160226181221735</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.4223265107215193</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.5933394048936181</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.4821817487607262</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.4386309850271404</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.4500210028016072</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>0.05383843622033489</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.4494780730940548</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.3804954911614504</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.4191340160140855</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.4290713633653567</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.6231555858102347</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.4811474376104958</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.4429254441760342</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.4557588483129089</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>0.05705615758781021</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.4663097078198372</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.3814394008346696</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.4104862511782502</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.4356979627862535</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.5637792110853987</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.5081264747546149</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.4391528551715386</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.4544317615138965</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>0.06046619009070436</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.4983581361543411</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.3992568940085459</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.4356406410923965</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.4480168366897399</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.5647285977499962</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.5092614878599598</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.4332530151634191</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.4669263850235558</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>0.06408002744416</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0.5152515426294753</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.4154469738806065</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.4636155882085594</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.4320341978661323</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.6269709949291425</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.5192110962032939</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.4308834384105747</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.4816565465483372</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>0.06790985029955714</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0.5251647414278513</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.4081148383885234</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.4658694946378064</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.4524252546024254</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.6279507540004742</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.5774604865942371</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.4329584712804895</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.493138628223681</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>0.07196856730011521</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0.54260180153582</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.4173970628847039</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.4319875812008784</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.4526432139638664</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.6333411715718734</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.6294999956980722</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.4401229983886891</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.4996178152020343</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>0.07626985859023444</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0.6094336685358277</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.4556858071515885</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.4332544777690713</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.4324235621622987</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.6583649227939395</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.6925455189766001</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.4351852105877294</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.5203097058169202</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>0.08082822192522715</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0.6717617681823368</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.4787863875374109</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.4163103468851494</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.4885104434176203</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.7111674763784332</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.7305946137514149</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.4452232910133844</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.5495181635120682</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0.08565902153685495</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.686664910676843</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.4971645254651021</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.448438253833177</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.4946518000739613</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.8218457090501089</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.8045914435293908</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.4724181091701008</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.5857410198029741</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>0.09077853991937558</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.702500386476428</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.5269466930204887</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.4668713483902664</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.5233220450217455</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.7969291948296883</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.7682740116081944</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.499221042369846</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.5989252314232115</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>0.09620403271064761</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.8372987290312888</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.5574542818600771</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.5090988896784165</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.5144017998648398</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.7560711503402666</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.7724166087234173</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.4958465932954296</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.6204517141377586</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>0.101953786853273</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.8877756773903104</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.5826452680347965</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.5212329151228854</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.595978132205729</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.7498634785212713</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.8526960455206097</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.5109050209432184</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.6563797557395671</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>0.1080471822318129</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.8017259189833876</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.6407141977836787</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.5449406635699692</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.6303972887060375</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.8450023041204821</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.9114557608070799</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.4893916166441427</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.6789587746592207</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>0.1145047569938282</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.9075773662873217</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.7012169655762927</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.5492644370704446</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.6644984062751743</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.8078140305701361</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.8818371872498509</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.5431984201648244</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.7088008937824216</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>0.1213482767749144</v>
+      </c>
+      <c r="B45" t="n">
+        <v>1.018209978110358</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.6732830647761978</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.5706368399607983</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.755971257486151</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.8864086078945792</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.7911754286711696</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.5629546749288111</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.7357907616975148</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>0.1286008080610566</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1.184205574748704</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.6084801118891582</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.5903592991984393</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.8331876868550295</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.9789450534880987</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.7598988204512372</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.551844971349161</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.7592925365162368</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>0.1362867959355774</v>
+      </c>
+      <c r="B47" t="n">
+        <v>1.19817451678198</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.7481512963301689</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.6262883004015452</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.9890929226954732</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.9630820682545455</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.8222724164693092</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.5327428436236508</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.8127549995302349</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>0.1444321464727281</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1.114713259186687</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.8003406758344466</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.6548378025848531</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.9677442949267844</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.8845664093967806</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.754086363351017</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.5602800982185877</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.8008581364605389</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>0.1530643140556359</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1.200810443359863</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.7321419882928613</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.6346152566912503</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.9496132128772313</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.8199396538119222</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.7683294661458997</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.6284032904131062</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.8000170916330158</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>0.1622123939129173</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.080030335760683</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1.008724513667065</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.7560095964257991</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.9539756987485852</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.8675583595339323</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.927350487695212</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.6931014336014975</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.8887953889632508</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>0.1719072201858575</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1.171836287629122</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.9991090329170768</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.7624045440068092</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.9237364202479951</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1.039760881128813</v>
+      </c>
+      <c r="G51" t="n">
+        <v>1.020483551917736</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.6701176127136943</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.9265566637149409</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>0.1821814698566975</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1.097207798925028</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1.025917785420161</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.7073196409810244</v>
+      </c>
+      <c r="E52" t="n">
+        <v>1.018534987757829</v>
+      </c>
+      <c r="F52" t="n">
+        <v>1.041591005350164</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.9898471293036805</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.6771460241384354</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.9219467294890257</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>0.1930697728883251</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1.053426223571824</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1.017466974439061</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.7750151299397284</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.9769298940921148</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.9383652152652792</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1.014405149542976</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.7401262591901924</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.9232354140449444</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>0.2046088289466012</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1.157239358743493</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1.021905889235557</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.7186725105301632</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.8824347394569311</v>
+      </c>
+      <c r="F54" t="n">
+        <v>1.045337578645613</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.9841443987466414</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.8086648313899242</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.934830979406192</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>0.2168375310987435</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1.193857776236342</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1.123471715263049</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.8138940511468939</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.963342287583553</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1.169396287970089</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.9770368821396068</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.850149493483854</v>
+      </c>
+      <c r="I55" t="n">
+        <v>1.003041133882933</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>0.2297970969046963</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.113113106364686</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1.137073823351055</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.8462143996556227</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.9745511993933964</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1.178936584565703</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1.109235645423004</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.8859095170552317</v>
+      </c>
+      <c r="I56" t="n">
+        <v>1.027514819179</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>0.2435312073433415</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1.190633322039445</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.9277774440685658</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.8296049253926226</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.9285271072634704</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.9023869833783071</v>
+      </c>
+      <c r="G57" t="n">
+        <v>1.078436157838367</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.9710662769133381</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.9693371130652065</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>0.2580861540418075</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1.199982670799279</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.8598445773244432</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.8570821197980134</v>
+      </c>
+      <c r="E58" t="n">
+        <v>1.000371915099543</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.9713128660024384</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1.029000273510991</v>
+      </c>
+      <c r="H58" t="n">
+        <v>1.042594041634854</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.9884453787148376</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>0.2735109953041209</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1.15194534866806</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.8943057448381647</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.9364667531287761</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.065117359577111</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.9981871556864474</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1.080083611949544</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.8362389934381262</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.9891410209783386</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>0.2898577214651068</v>
+      </c>
+      <c r="B60" t="n">
+        <v>1.097583595219825</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.9682047356337919</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.8936521157079954</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1.008230775342019</v>
+      </c>
+      <c r="F60" t="n">
+        <v>1.092930393135653</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.8992455553916221</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.8946590730206034</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.9757152407817737</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>0.3071814301268697</v>
+      </c>
+      <c r="B61" t="n">
+        <v>1.052711102765725</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1.056719762546333</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.9216704742046852</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.9334101562699164</v>
+      </c>
+      <c r="F61" t="n">
+        <v>1.021382276412084</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.9486042016928564</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.9271607223916616</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.9786351318948137</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>0.3255405118685032</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0.9968337164306237</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.9982035866605824</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1.078443875417128</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.9512274316089083</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.8374092024369306</v>
+      </c>
+      <c r="G62" t="n">
+        <v>1.029528367509228</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.9797155043548256</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.9790389488734564</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>0.3449968470549717</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.9069341309930634</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.8866026054187401</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1.061223343184217</v>
+      </c>
+      <c r="E63" t="n">
+        <v>1.027149610571972</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.899549901844348</v>
+      </c>
+      <c r="G63" t="n">
+        <v>1.005500308424322</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.9469353375244732</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.9598656155028754</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>0.3656160144085195</v>
+      </c>
+      <c r="B64" t="n">
+        <v>1.055947880193224</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1.020642446906245</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.9449128962194978</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1.010134901185516</v>
+      </c>
+      <c r="F64" t="n">
+        <v>1.02311443717401</v>
+      </c>
+      <c r="G64" t="n">
+        <v>1.094875347460333</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.9356144585840667</v>
+      </c>
+      <c r="I64" t="n">
+        <v>1.010805467445131</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>0.3874675120456132</v>
+      </c>
+      <c r="B65" t="n">
+        <v>1.125563303584175</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1.042774035487877</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.9973341765178158</v>
+      </c>
+      <c r="E65" t="n">
+        <v>1.099803270452958</v>
+      </c>
+      <c r="F65" t="n">
+        <v>1.009061410875369</v>
+      </c>
+      <c r="G65" t="n">
+        <v>1.260586949648007</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0.9257915990241635</v>
+      </c>
+      <c r="I65" t="n">
+        <v>1.061248450147469</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>0.4106249917244298</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.433748131449705</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1.041211163550372</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.9592929860373764</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.9653421985376314</v>
+      </c>
+      <c r="F66" t="n">
+        <v>1.188560156325682</v>
+      </c>
+      <c r="G66" t="n">
+        <v>1.174158407496444</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0.8873602973850971</v>
+      </c>
+      <c r="I66" t="n">
+        <v>1.079831552774157</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>0.4351665070924416</v>
+      </c>
+      <c r="B67" t="n">
+        <v>1.402385758523872</v>
+      </c>
+      <c r="C67" t="n">
+        <v>1.142846074355476</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1.056101235951816</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.8945840755818437</v>
+      </c>
+      <c r="F67" t="n">
+        <v>1.318576960930211</v>
+      </c>
+      <c r="G67" t="n">
+        <v>1.171327176385093</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0.9328017745571564</v>
+      </c>
+      <c r="I67" t="n">
+        <v>1.117875848560036</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>0.4611747767708259</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.412020533220761</v>
+      </c>
+      <c r="C68" t="n">
+        <v>1.173953020319757</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1.068193437098487</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.9443050124150449</v>
+      </c>
+      <c r="F68" t="n">
+        <v>1.288694620447286</v>
+      </c>
+      <c r="G68" t="n">
+        <v>1.24221712056519</v>
+      </c>
+      <c r="H68" t="n">
+        <v>1.041561753237121</v>
+      </c>
+      <c r="I68" t="n">
+        <v>1.157743507756492</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>0.4887374631624425</v>
+      </c>
+      <c r="B69" t="n">
+        <v>1.272983870678634</v>
+      </c>
+      <c r="C69" t="n">
+        <v>1.134886263203732</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1.050457818721862</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.9336962045923557</v>
+      </c>
+      <c r="F69" t="n">
+        <v>1.006785472003532</v>
+      </c>
+      <c r="G69" t="n">
+        <v>1.08923267709284</v>
+      </c>
+      <c r="H69" t="n">
+        <v>1.121780320743768</v>
+      </c>
+      <c r="I69" t="n">
+        <v>1.082617346698643</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>0.5179474679231213</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1.11755407503295</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1.11763174872886</v>
+      </c>
+      <c r="D70" t="n">
+        <v>1.075287510181229</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1.110519128561678</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.9803325372244217</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.9311529511981347</v>
+      </c>
+      <c r="H70" t="n">
+        <v>1.294641761744582</v>
+      </c>
+      <c r="I70" t="n">
+        <v>1.084341292765944</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>0.5489032450921557</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1.067316869523805</v>
+      </c>
+      <c r="C71" t="n">
+        <v>1.072854481238496</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1.160159964395971</v>
+      </c>
+      <c r="E71" t="n">
+        <v>1.048754723357365</v>
+      </c>
+      <c r="F71" t="n">
+        <v>1.004483019514341</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.9140458798207084</v>
+      </c>
+      <c r="H71" t="n">
+        <v>1.540223333385381</v>
+      </c>
+      <c r="I71" t="n">
+        <v>1.101727848448245</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>0.5817091329374358</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1.084295542796534</v>
+      </c>
+      <c r="C72" t="n">
+        <v>1.054870904524927</v>
+      </c>
+      <c r="D72" t="n">
+        <v>1.146198615464379</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1.063260535022791</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.9762750824297161</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0.8907913212909098</v>
+      </c>
+      <c r="H72" t="n">
+        <v>1.68495258160279</v>
+      </c>
+      <c r="I72" t="n">
+        <v>1.107418501929604</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>0.6164757056337165</v>
+      </c>
+      <c r="B73" t="n">
+        <v>1.155926125583469</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.9532281516639857</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.9993957658634384</v>
+      </c>
+      <c r="E73" t="n">
+        <v>1.149076401002445</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.9482376167017407</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.815268900459924</v>
+      </c>
+      <c r="H73" t="n">
+        <v>1.687379760122914</v>
+      </c>
+      <c r="I73" t="n">
+        <v>1.07421703326713</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>0.6533201459593774</v>
+      </c>
+      <c r="B74" t="n">
+        <v>1.064246642425038</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1.242632998478711</v>
+      </c>
+      <c r="D74" t="n">
+        <v>1.094110684777676</v>
+      </c>
+      <c r="E74" t="n">
+        <v>1.05857945007342</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.969338970757407</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.880632560339317</v>
+      </c>
+      <c r="H74" t="n">
+        <v>1.563387521557438</v>
+      </c>
+      <c r="I74" t="n">
+        <v>1.107536721589644</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>0.6923666402678728</v>
+      </c>
+      <c r="B75" t="n">
+        <v>1.100892320397702</v>
+      </c>
+      <c r="C75" t="n">
+        <v>1.200755922400234</v>
+      </c>
+      <c r="D75" t="n">
+        <v>1.103350618187021</v>
+      </c>
+      <c r="E75" t="n">
+        <v>1.061824194033832</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.9355034250315793</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.8446346610742137</v>
+      </c>
+      <c r="H75" t="n">
+        <v>1.490378479622246</v>
+      </c>
+      <c r="I75" t="n">
+        <v>1.089638325569043</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>0.7337467970651381</v>
+      </c>
+      <c r="B76" t="n">
+        <v>1.024329582397531</v>
+      </c>
+      <c r="C76" t="n">
+        <v>1.017976957022626</v>
+      </c>
+      <c r="D76" t="n">
+        <v>1.038652350521553</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.9351408855454589</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.9621253996809563</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.8881216614252192</v>
+      </c>
+      <c r="H76" t="n">
+        <v>1.23287461804458</v>
+      </c>
+      <c r="I76" t="n">
+        <v>1.009302011158719</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>0.7776000906038036</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0.9978567935246746</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.835356886633528</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.8658997647243835</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.9090179394968911</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.9325094401423397</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.9206728526728356</v>
+      </c>
+      <c r="H77" t="n">
+        <v>1.110741569097883</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0.9352062953939473</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>0.8240743309893661</v>
+      </c>
+      <c r="B78" t="n">
+        <v>1.007139049140124</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.8828983543293965</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.8763507356137162</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.9784959401950781</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.8741971577083536</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.9985541763473319</v>
+      </c>
+      <c r="H78" t="n">
+        <v>1.164600684110081</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0.9642714596089598</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>0.8733261623828433</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0.9814441797586013</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.9158494904247054</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.89287232906051</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.8569229136168124</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.806786783494013</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0.9324610185594724</v>
+      </c>
+      <c r="H79" t="n">
+        <v>1.021400636780909</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0.9129132028928676</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>0.9255215909791353</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0.853923389497656</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.8597567587467752</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.8827607449210166</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.8155039754194221</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.8320370829958179</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0.8580699076407974</v>
+      </c>
+      <c r="H80" t="n">
+        <v>1.093289633979239</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0.8811834108150571</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>0.980836544540667</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0.9169878955303927</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.8535133620067442</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.8653824379932877</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.8691074767544537</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.83895259371192</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.8060941930388117</v>
+      </c>
+      <c r="H81" t="n">
+        <v>1.056235920148891</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0.8835853765233345</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>1.039457465372263</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0.9979194677328331</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.835173718615047</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.8624772052597919</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.9148783825102099</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.7716010971548962</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0.7422961435926132</v>
+      </c>
+      <c r="H82" t="n">
+        <v>1.264151226264512</v>
+      </c>
+      <c r="I82" t="n">
+        <v>0.8994243175295645</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>1.1015819387359</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0.8571634655676887</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.7775933613925244</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.894988439365762</v>
+      </c>
+      <c r="E83" t="n">
+        <v>1.004434473454397</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.9086465621383194</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0.7567652345203892</v>
+      </c>
+      <c r="H83" t="n">
+        <v>1.265552091286589</v>
+      </c>
+      <c r="I83" t="n">
+        <v>0.9111686607668444</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>1.167419358823459</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0.8066452530577147</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.6993464485435266</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.8732148468569478</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.9624394553456711</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.9821130573306761</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0.7901140126374705</v>
+      </c>
+      <c r="H84" t="n">
+        <v>1.007287425815645</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0.8677819101302332</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>1.237191634532161</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0.6762619257006088</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.6434192091391747</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0.8483403436499404</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.8377097523388147</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0.8752425784376865</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0.7384940535209208</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0.7489778863585234</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0.7623841688898996</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>1.311133937421564</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0.6454420238753805</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.6040201604666859</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.8399897989541855</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.6218109221883238</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0.7383451789370925</v>
+      </c>
+      <c r="G86" t="n">
+        <v>0.6247572945956953</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0.6440553492400565</v>
+      </c>
+      <c r="I86" t="n">
+        <v>0.6698262189338057</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>1.389495494373137</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0.7508447935560627</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.5575481375759689</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.7405107688803644</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.5208266530635461</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0.7173292783946353</v>
+      </c>
+      <c r="G87" t="n">
+        <v>0.5368433052483838</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0.6654520251603823</v>
+      </c>
+      <c r="I87" t="n">
+        <v>0.6344412683262499</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>1.472540427624122</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.6567165351046866</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.6076029841676311</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.6332132091369441</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.5151087674224092</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0.7059739815424992</v>
+      </c>
+      <c r="G88" t="n">
+        <v>0.5704770736327518</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0.6715532068401926</v>
+      </c>
+      <c r="I88" t="n">
+        <v>0.6199617106826406</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>1.560548645007075</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.5630660819125287</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.6001926148327921</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.5433339757014373</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.4545193635843567</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0.6419724120757662</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0.4939283081844495</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0.6491726641050015</v>
+      </c>
+      <c r="I89" t="n">
+        <v>0.5595753037316082</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>1.653816783395673</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0.4185433722847666</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0.5697748362041001</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.5018009542631786</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.4024005003440746</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0.5580593649303024</v>
+      </c>
+      <c r="G90" t="n">
+        <v>0.4466403380554426</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0.5479851239138429</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0.4878558856913235</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>1.752659208536758</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0.3707426188379665</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.4803421020430014</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.4688813108682948</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.3939521477852401</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0.4965242153821482</v>
+      </c>
+      <c r="G91" t="n">
+        <v>0.4265891348580269</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0.5437857030130703</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0.45089197960536</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>1.857409074638572</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0.4761481581336071</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0.420169478577276</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.449255819273465</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0.3479708757697264</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0.4567920971714666</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0.4136759762707257</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0.4486517631391231</v>
+      </c>
+      <c r="I92" t="n">
+        <v>0.4284768416718781</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>1.968419447286611</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0.5274047686630373</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0.3919678275850284</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.3913286377957655</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.3334425337534033</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0.410048683134101</v>
+      </c>
+      <c r="G93" t="n">
+        <v>0.4057868992178618</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0.3855415117806699</v>
+      </c>
+      <c r="I93" t="n">
+        <v>0.4031360816409111</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>2.086064493471959</v>
+      </c>
+      <c r="B94" t="n">
+        <v>0.4366244767879927</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0.3503008376928857</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.3473749106453752</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.3331552406601961</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0.3396087235865618</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0.360346946889993</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0.3730035893413207</v>
+      </c>
+      <c r="I94" t="n">
+        <v>0.3615771744747732</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>2.210740742743126</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0.4161952055891283</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0.3320178313711232</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.3516996177239265</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.2956902234489001</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0.3021545358809456</v>
+      </c>
+      <c r="G95" t="n">
+        <v>0.3445027265757643</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0.3771988713792905</v>
+      </c>
+      <c r="I95" t="n">
+        <v>0.3434968723988054</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>2.342868423732233</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0.3743838222879213</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0.3083664088012822</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.3318005255143353</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.3491886661311298</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0.2758898415611951</v>
+      </c>
+      <c r="G96" t="n">
+        <v>0.3466934920078149</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0.3211538766603051</v>
+      </c>
+      <c r="I96" t="n">
+        <v>0.3282805334656033</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>2.482892880560327</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0.3169470182541949</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0.2935564996372838</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0.3036826787140295</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0.2974141687237583</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0.2880393955209922</v>
+      </c>
+      <c r="G97" t="n">
+        <v>0.3396451020122506</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0.2698620079988771</v>
+      </c>
+      <c r="I97" t="n">
+        <v>0.3006154461345349</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>2.631286073895945</v>
+      </c>
+      <c r="B98" t="n">
+        <v>0.2840204041430114</v>
+      </c>
+      <c r="C98" t="n">
+        <v>0.2873194823474377</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0.2707257855539194</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0.2283268860099477</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0.2643207864489594</v>
+      </c>
+      <c r="G98" t="n">
+        <v>0.3036580633720964</v>
+      </c>
+      <c r="H98" t="n">
+        <v>0.2977773305952625</v>
+      </c>
+      <c r="I98" t="n">
+        <v>0.2755324303608701</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>2.788548171726292</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0.258611147414159</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0.2293769901892944</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0.2729023294799479</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.234461271949989</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0.2566206967179159</v>
+      </c>
+      <c r="G99" t="n">
+        <v>0.2867764822192562</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0.3087259608375599</v>
+      </c>
+      <c r="I99" t="n">
+        <v>0.2626536267913576</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>2.955209235202888</v>
+      </c>
+      <c r="B100" t="n">
+        <v>0.2346792157517953</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0.2146939076068997</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0.2285115321937155</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0.2211462702395744</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0.2475265259654801</v>
+      </c>
+      <c r="G100" t="n">
+        <v>0.2678388198314409</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0.2489072412607532</v>
+      </c>
+      <c r="I100" t="n">
+        <v>0.237013757724274</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>3.131831005243845</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0.2282089906586028</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0.1953678300606285</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.244909566582171</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.2328842874239037</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0.248507047458907</v>
+      </c>
+      <c r="G101" t="n">
+        <v>0.2361208936954213</v>
+      </c>
+      <c r="H101" t="n">
+        <v>0.2073779852540671</v>
+      </c>
+      <c r="I101" t="n">
+        <v>0.226879554068015</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>3.319008795914677</v>
+      </c>
+      <c r="B102" t="n">
+        <v>0.1856372391338881</v>
+      </c>
+      <c r="C102" t="n">
+        <v>0.2086792841743549</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.2241038922627598</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0.2189924278204235</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0.2489037559026034</v>
+      </c>
+      <c r="G102" t="n">
+        <v>0.2094004421186771</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0.1844884868711936</v>
+      </c>
+      <c r="I102" t="n">
+        <v>0.2104471437448207</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>3.517373500969384</v>
+      </c>
+      <c r="B103" t="n">
+        <v>0.1591838375657398</v>
+      </c>
+      <c r="C103" t="n">
+        <v>0.2092132908337391</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0.1947554028428732</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.2286017158358423</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0.2225953234499995</v>
+      </c>
+      <c r="G103" t="n">
+        <v>0.198494242999927</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0.1911863338589121</v>
+      </c>
+      <c r="I103" t="n">
+        <v>0.1993804522975336</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>3.727593720314942</v>
+      </c>
+      <c r="B104" t="n">
+        <v>0.1640406997071582</v>
+      </c>
+      <c r="C104" t="n">
+        <v>0.1964874235680874</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0.1761633043798325</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.2082991156222356</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0.1980639257455002</v>
+      </c>
+      <c r="G104" t="n">
+        <v>0.2013737867767026</v>
+      </c>
+      <c r="H104" t="n">
+        <v>0.2140123333729934</v>
+      </c>
+      <c r="I104" t="n">
+        <v>0.1933326461933645</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>3.950378013566644</v>
+      </c>
+      <c r="B105" t="n">
+        <v>0.1641376362307003</v>
+      </c>
+      <c r="C105" t="n">
+        <v>0.1867063571867129</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0.1823346288924081</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0.1831559908835379</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0.1769974563906014</v>
+      </c>
+      <c r="G105" t="n">
+        <v>0.1827883167180004</v>
+      </c>
+      <c r="H105" t="n">
+        <v>0.2261093424467549</v>
+      </c>
+      <c r="I105" t="n">
+        <v>0.1852490259726961</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>4.186477288289951</v>
+      </c>
+      <c r="B106" t="n">
+        <v>0.1723164336797686</v>
+      </c>
+      <c r="C106" t="n">
+        <v>0.2187626898155923</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0.1490304291284485</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.1661371893131829</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0.1728449633477745</v>
+      </c>
+      <c r="G106" t="n">
+        <v>0.1655862693309913</v>
+      </c>
+      <c r="H106" t="n">
+        <v>0.2113135303117018</v>
+      </c>
+      <c r="I106" t="n">
+        <v>0.1779244906878292</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>4.436687330978611</v>
+      </c>
+      <c r="B107" t="n">
+        <v>0.1736436705109304</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0.254635225104744</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0.1299804650779262</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0.1555839916245449</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0.1684648172911526</v>
+      </c>
+      <c r="G107" t="n">
+        <v>0.1534572696484975</v>
+      </c>
+      <c r="H107" t="n">
+        <v>0.1859317985764523</v>
+      </c>
+      <c r="I107" t="n">
+        <v>0.1711293096062516</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>4.701851489299856</v>
+      </c>
+      <c r="B108" t="n">
+        <v>0.1666200203343761</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0.2071686303705585</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0.1290103996589488</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0.1552643811702789</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0.1608798532964956</v>
+      </c>
+      <c r="G108" t="n">
+        <v>0.2084724188323819</v>
+      </c>
+      <c r="H108" t="n">
+        <v>0.1929051133350839</v>
+      </c>
+      <c r="I108" t="n">
+        <v>0.1721099439351335</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>4.982863514647306</v>
+      </c>
+      <c r="B109" t="n">
+        <v>0.1755017398360185</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0.1445537666584187</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0.1464116025889878</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0.1605728928251572</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0.1506776187258375</v>
+      </c>
+      <c r="G109" t="n">
+        <v>0.1852928888606121</v>
+      </c>
+      <c r="H109" t="n">
+        <v>0.189555964226523</v>
+      </c>
+      <c r="I109" t="n">
+        <v>0.163746464307048</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>5.280670574582637</v>
+      </c>
+      <c r="B110" t="n">
+        <v>0.1714316661776543</v>
+      </c>
+      <c r="C110" t="n">
+        <v>0.1335520002639711</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0.1588001525362015</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0.1464202226265547</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0.1382194549734348</v>
+      </c>
+      <c r="G110" t="n">
+        <v>0.1831506228096018</v>
+      </c>
+      <c r="H110" t="n">
+        <v>0.1726318274730588</v>
+      </c>
+      <c r="I110" t="n">
+        <v>0.1567623246371299</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>5.596276445319552</v>
+      </c>
+      <c r="B111" t="n">
+        <v>0.1340802654181888</v>
+      </c>
+      <c r="C111" t="n">
+        <v>0.1157370044114477</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0.1427611878353512</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0.1301717707853018</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0.1275947140849178</v>
+      </c>
+      <c r="G111" t="n">
+        <v>0.1930807349307852</v>
+      </c>
+      <c r="H111" t="n">
+        <v>0.1477889414435533</v>
+      </c>
+      <c r="I111" t="n">
+        <v>0.1399208769481277</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>5.930744895010559</v>
+      </c>
+      <c r="B112" t="n">
+        <v>0.1110343226892554</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0.1060034727137684</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0.1187751553234922</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0.1162215003135428</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0.1307835055993175</v>
+      </c>
+      <c r="G112" t="n">
+        <v>0.2067666160914644</v>
+      </c>
+      <c r="H112" t="n">
+        <v>0.1164174816911149</v>
+      </c>
+      <c r="I112" t="n">
+        <v>0.1262591911838389</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>6.285203269240103</v>
+      </c>
+      <c r="B113" t="n">
+        <v>0.1080860831257321</v>
+      </c>
+      <c r="C113" t="n">
+        <v>0.09689336111568744</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0.1088227929248345</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0.1079603379387329</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0.1315547655670435</v>
+      </c>
+      <c r="G113" t="n">
+        <v>0.2050457671838912</v>
+      </c>
+      <c r="H113" t="n">
+        <v>0.115739486173166</v>
+      </c>
+      <c r="I113" t="n">
+        <v>0.1211987444983255</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>6.660846290809161</v>
+      </c>
+      <c r="B114" t="n">
+        <v>0.1027338566774523</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0.0909117474479411</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0.1036681660561249</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0.09657817737746437</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0.1231527340404056</v>
+      </c>
+      <c r="G114" t="n">
+        <v>0.1773601514730677</v>
+      </c>
+      <c r="H114" t="n">
+        <v>0.1053075369371286</v>
+      </c>
+      <c r="I114" t="n">
+        <v>0.1115621300094885</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>7.058940086618745</v>
+      </c>
+      <c r="B115" t="n">
+        <v>0.09138033362366035</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0.08007953439170185</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0.09666850105630252</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0.080812019750011</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0.1092316690027861</v>
+      </c>
+      <c r="G115" t="n">
+        <v>0.1495503854377913</v>
+      </c>
+      <c r="H115" t="n">
+        <v>0.08735781020862597</v>
+      </c>
+      <c r="I115" t="n">
+        <v>0.09713317423846508</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>7.480826455225086</v>
+      </c>
+      <c r="B116" t="n">
+        <v>0.0715125707383311</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0.07071753564894023</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0.08985559057073596</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0.07973560422855999</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0.09958327962562394</v>
+      </c>
+      <c r="G116" t="n">
+        <v>0.1307103908763441</v>
+      </c>
+      <c r="H116" t="n">
+        <v>0.07347867838624651</v>
+      </c>
+      <c r="I116" t="n">
+        <v>0.08595123292820665</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>7.927927389450597</v>
+      </c>
+      <c r="B117" t="n">
+        <v>0.05847814035897755</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0.0655173501701293</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0.08390011708911332</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0.1011825455484528</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0.08724238105936485</v>
+      </c>
+      <c r="G117" t="n">
+        <v>0.1112996922573147</v>
+      </c>
+      <c r="H117" t="n">
+        <v>0.06475302590952513</v>
+      </c>
+      <c r="I117" t="n">
+        <v>0.0797128822206685</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>8.401749869294344</v>
+      </c>
+      <c r="B118" t="n">
+        <v>0.04632838023402208</v>
+      </c>
+      <c r="C118" t="n">
+        <v>0.0619270150555821</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0.07486639551708854</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0.09639285434959155</v>
+      </c>
+      <c r="F118" t="n">
+        <v>0.07296487591238709</v>
+      </c>
+      <c r="G118" t="n">
+        <v>0.09147837488125883</v>
+      </c>
+      <c r="H118" t="n">
+        <v>0.05773878931190227</v>
+      </c>
+      <c r="I118" t="n">
+        <v>0.06968463003307981</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>8.903890941296735</v>
+      </c>
+      <c r="B119" t="n">
+        <v>0.03575617645172337</v>
+      </c>
+      <c r="C119" t="n">
+        <v>0.05765589924849306</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0.06620118833086955</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0.08599764919065603</v>
+      </c>
+      <c r="F119" t="n">
+        <v>0.0609643482428557</v>
+      </c>
+      <c r="G119" t="n">
+        <v>0.07347611104653794</v>
+      </c>
+      <c r="H119" t="n">
+        <v>0.04988497428094472</v>
+      </c>
+      <c r="I119" t="n">
+        <v>0.05944366481288383</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>9.436043101478891</v>
+      </c>
+      <c r="B120" t="n">
+        <v>0.02812757546183784</v>
+      </c>
+      <c r="C120" t="n">
+        <v>0.04951309901406587</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0.05825442393273553</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0.06815900269354452</v>
+      </c>
+      <c r="F120" t="n">
+        <v>0.05086157863636179</v>
+      </c>
+      <c r="G120" t="n">
+        <v>0.06134084861111864</v>
+      </c>
+      <c r="H120" t="n">
+        <v>0.04182693904589575</v>
+      </c>
+      <c r="I120" t="n">
+        <v>0.04943595091037688</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
         <v>10</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B121" t="n">
         <v>0.02389384167686914</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C121" t="n">
         <v>0.04420608497401755</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D121" t="n">
         <v>0.05197121008776968</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E121" t="n">
         <v>0.05581094280546197</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F121" t="n">
         <v>0.04468867093096585</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G121" t="n">
         <v>0.04972301404441996</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H121" t="n">
         <v>0.03509016963223178</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I121" t="n">
         <v>0.04221393106802819</v>
       </c>
     </row>

</xml_diff>